<commit_message>
remove literatures/ and ~$input.xlsx
</commit_message>
<xml_diff>
--- a/experiments/fluorescence_protein/input_ecoli2/input_AzG.xlsx
+++ b/experiments/fluorescence_protein/input_ecoli2/input_AzG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOFKV\PycharmProjects\proseqteleporter\experiments\fluorescence_protein\input_ecoli2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOFKV\PycharmProjects\seqTeleporter\experiments\fluorescence_protein\input_ecoli2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48DE688-B2CB-4FDF-95A5-F7A437C1546B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BA1582-61EC-4911-BB2F-673CA06D760F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="768" activeTab="5" xr2:uid="{92EDD624-EB72-41A1-9013-2A2A4F6AE6A6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="768" activeTab="3" xr2:uid="{92EDD624-EB72-41A1-9013-2A2A4F6AE6A6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_guide" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="221">
   <si>
     <t>SEQUENCE</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>Q63H,R67K,F80L,S143I,V158N,F174I,H194Y</t>
+  </si>
+  <si>
+    <t>(62,66),(102,106),(142,146),(182,185)</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B18F55-B802-4234-9243-47420B950F19}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1722,6 +1725,9 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
@@ -1736,7 +1742,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1785,7 +1791,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1987,14 +1993,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEB98E8-6985-45FF-840E-89664040D491}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B97"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>